<commit_message>
Updated UI and other misc. stuff
</commit_message>
<xml_diff>
--- a/data/Text Props.xlsx
+++ b/data/Text Props.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdebe\Documents\GitHub\Climate_Obstruction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E82B93-AE76-4163-86D8-43DA9E138C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57D560F-9808-47F6-B693-D29870B0709D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20730" yWindow="405" windowWidth="7050" windowHeight="14070" xr2:uid="{9DCCEFF8-3E6C-467C-844F-F92DAC5948FD}"/>
+    <workbookView xWindow="13230" yWindow="840" windowWidth="6315" windowHeight="14070" xr2:uid="{9DCCEFF8-3E6C-467C-844F-F92DAC5948FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,10 +108,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -146,6 +153,7 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,13 +507,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428A9199-1DD7-4253-873F-AEDAE862C70B}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +529,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +545,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +561,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +585,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +593,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +601,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +609,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +617,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +633,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +649,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,7 +665,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,15 +673,15 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +689,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added files for Allen Time Interval
</commit_message>
<xml_diff>
--- a/data/Text Props.xlsx
+++ b/data/Text Props.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdebe\Documents\GitHub\Climate_Obstruction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57D560F-9808-47F6-B693-D29870B0709D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DF8050-93CD-4B2C-8B59-1F896496EC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="840" windowWidth="6315" windowHeight="14070" xr2:uid="{9DCCEFF8-3E6C-467C-844F-F92DAC5948FD}"/>
+    <workbookView xWindow="780" yWindow="570" windowWidth="5535" windowHeight="14910" xr2:uid="{9DCCEFF8-3E6C-467C-844F-F92DAC5948FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>at_issue</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>members</t>
+  </si>
+  <si>
+    <t>funds</t>
+  </si>
+  <si>
+    <t>funding_received</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428A9199-1DD7-4253-873F-AEDAE862C70B}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +535,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +543,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,7 +551,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,7 +567,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +591,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +599,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,100 +607,116 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
+      <c r="A21" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="1" t="b">
-        <v>1</v>
+      <c r="B24" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A21">
-    <sortCondition ref="A1:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A24">
+    <sortCondition ref="A1:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>